<commit_message>
Update pptx bionica automations and rubrikas repo to lattest commit
</commit_message>
<xml_diff>
--- a/fol/Concurso/Anexos/Anexo 2 - Esquema de conexiones/UBALDE_Esquema_conexiones.xlsx
+++ b/fol/Concurso/Anexos/Anexo 2 - Esquema de conexiones/UBALDE_Esquema_conexiones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dani\repos\2h\fol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kerjox\Repos\2h\fol\Concurso\Anexos\Anexo 2 - Esquema de conexiones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA79323-69BA-4E3A-B94C-346C38ACFE14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6C983D-6E84-4FF9-A3E4-C228AA840E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="300" windowWidth="23256" windowHeight="13644" xr2:uid="{47CFAA2B-B6FE-4C8E-9BA2-DB30D79CCD5C}"/>
+    <workbookView xWindow="-120" yWindow="285" windowWidth="38640" windowHeight="20865" xr2:uid="{47CFAA2B-B6FE-4C8E-9BA2-DB30D79CCD5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Conexiones" sheetId="1" r:id="rId1"/>
@@ -1210,26 +1210,26 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" customWidth="1"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>114</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>63</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>63</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>73</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>64</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>64</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>64</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>64</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>64</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>64</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>64</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>64</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>64</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>64</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>64</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>64</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>64</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>64</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>64</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>64</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>64</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>64</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>64</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>64</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>64</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>64</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>64</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>64</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>64</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>64</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>64</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>64</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>65</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>65</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>65</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>65</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>65</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>65</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>65</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>65</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>65</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>65</v>
       </c>
@@ -2350,7 +2350,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>65</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>65</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>65</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>65</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>65</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>65</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>65</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>65</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>65</v>
       </c>
@@ -2584,7 +2584,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>65</v>
       </c>
@@ -2610,7 +2610,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>65</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>65</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>65</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>65</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>65</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>65</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>65</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>65</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>66</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>66</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>66</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>66</v>
       </c>
@@ -2922,7 +2922,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>66</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>66</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>66</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>66</v>
       </c>
@@ -3026,7 +3026,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>66</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>66</v>
       </c>
@@ -3078,7 +3078,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>66</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>66</v>
       </c>
@@ -3130,7 +3130,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>66</v>
       </c>
@@ -3156,7 +3156,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>66</v>
       </c>
@@ -3182,7 +3182,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>66</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>66</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>66</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>66</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>66</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>66</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>66</v>
       </c>
@@ -3360,7 +3360,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>66</v>
       </c>
@@ -3386,7 +3386,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>66</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>66</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>66</v>
       </c>
@@ -3464,7 +3464,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>66</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>66</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>66</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>67</v>
       </c>
@@ -3568,7 +3568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>67</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>67</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>67</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>67</v>
       </c>
@@ -3672,7 +3672,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>67</v>
       </c>
@@ -3698,7 +3698,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="97" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>67</v>
       </c>
@@ -3724,7 +3724,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>67</v>
       </c>
@@ -3750,7 +3750,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>67</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>67</v>
       </c>
@@ -3802,7 +3802,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>67</v>
       </c>
@@ -3828,7 +3828,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="102" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>67</v>
       </c>
@@ -3854,7 +3854,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>67</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="104" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>67</v>
       </c>
@@ -3906,7 +3906,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="105" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>67</v>
       </c>
@@ -3932,7 +3932,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>67</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="107" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>67</v>
       </c>
@@ -3984,7 +3984,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="108" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>67</v>
       </c>
@@ -4010,7 +4010,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="109" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>67</v>
       </c>
@@ -4036,7 +4036,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="110" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>67</v>
       </c>
@@ -4062,7 +4062,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="111" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>67</v>
       </c>
@@ -4088,7 +4088,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="112" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>67</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="113" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>67</v>
       </c>
@@ -4140,7 +4140,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="114" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>67</v>
       </c>
@@ -4166,7 +4166,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="115" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>67</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="116" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>67</v>
       </c>
@@ -4218,7 +4218,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="117" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>67</v>
       </c>
@@ -4244,7 +4244,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="118" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>67</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="119" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>68</v>
       </c>
@@ -4296,7 +4296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>68</v>
       </c>
@@ -4322,7 +4322,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>68</v>
       </c>
@@ -4348,7 +4348,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="122" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>68</v>
       </c>
@@ -4374,7 +4374,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>68</v>
       </c>
@@ -4400,7 +4400,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>68</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="125" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>68</v>
       </c>
@@ -4452,7 +4452,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="126" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>68</v>
       </c>
@@ -4478,7 +4478,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="127" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>68</v>
       </c>
@@ -4504,7 +4504,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>68</v>
       </c>
@@ -4530,7 +4530,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>68</v>
       </c>
@@ -4556,7 +4556,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="130" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>68</v>
       </c>
@@ -4582,7 +4582,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="131" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>68</v>
       </c>
@@ -4608,7 +4608,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="132" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>68</v>
       </c>
@@ -4634,7 +4634,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="133" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>68</v>
       </c>
@@ -4660,7 +4660,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="134" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>68</v>
       </c>
@@ -4686,7 +4686,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="135" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>68</v>
       </c>
@@ -4712,7 +4712,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="136" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
         <v>68</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="137" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>68</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="138" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
         <v>68</v>
       </c>
@@ -4790,7 +4790,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="139" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>68</v>
       </c>
@@ -4816,7 +4816,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="140" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>68</v>
       </c>
@@ -4842,7 +4842,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="141" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>68</v>
       </c>
@@ -4868,7 +4868,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="142" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>68</v>
       </c>
@@ -4894,7 +4894,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="143" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
         <v>68</v>
       </c>
@@ -4920,7 +4920,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="144" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
         <v>68</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="145" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
         <v>68</v>
       </c>
@@ -4972,7 +4972,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="146" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
         <v>68</v>
       </c>
@@ -4998,7 +4998,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="147" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
         <v>131</v>
       </c>
@@ -5024,7 +5024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
         <v>131</v>
       </c>
@@ -5050,7 +5050,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="149" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
         <v>131</v>
       </c>
@@ -5076,7 +5076,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="150" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>131</v>
       </c>
@@ -5102,7 +5102,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="151" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
         <v>131</v>
       </c>
@@ -5128,7 +5128,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="152" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>131</v>
       </c>
@@ -5154,7 +5154,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="153" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
         <v>131</v>
       </c>
@@ -5180,7 +5180,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="154" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
         <v>131</v>
       </c>
@@ -5206,7 +5206,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="155" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
         <v>131</v>
       </c>
@@ -5232,7 +5232,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="156" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
         <v>131</v>
       </c>
@@ -5258,7 +5258,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="157" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
         <v>131</v>
       </c>
@@ -5284,7 +5284,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="158" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
         <v>131</v>
       </c>
@@ -5310,7 +5310,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="159" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
         <v>131</v>
       </c>
@@ -5336,7 +5336,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="160" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
         <v>131</v>
       </c>
@@ -5362,7 +5362,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="161" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
         <v>131</v>
       </c>
@@ -5388,7 +5388,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="162" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
         <v>131</v>
       </c>
@@ -5414,7 +5414,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="163" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
         <v>131</v>
       </c>
@@ -5440,7 +5440,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="164" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
         <v>131</v>
       </c>
@@ -5466,7 +5466,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="165" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
         <v>131</v>
       </c>
@@ -5492,7 +5492,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="166" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
         <v>131</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="167" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
         <v>131</v>
       </c>
@@ -5544,7 +5544,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="168" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
         <v>131</v>
       </c>
@@ -5570,7 +5570,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="169" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
         <v>131</v>
       </c>
@@ -5596,7 +5596,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="170" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
         <v>131</v>
       </c>
@@ -5622,7 +5622,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="171" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
         <v>131</v>
       </c>
@@ -5648,7 +5648,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="172" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
         <v>131</v>
       </c>
@@ -5674,7 +5674,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="173" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
         <v>131</v>
       </c>
@@ -5700,7 +5700,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="174" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
         <v>131</v>
       </c>
@@ -5744,18 +5744,18 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
@@ -5778,7 +5778,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="3:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C6" s="3">
         <v>10</v>
       </c>
@@ -5801,7 +5801,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="3:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C7" s="3">
         <v>20</v>
       </c>
@@ -5824,7 +5824,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="3:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C8" s="3">
         <v>30</v>
       </c>
@@ -5847,7 +5847,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="3:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C9" s="3">
         <v>40</v>
       </c>
@@ -5870,7 +5870,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="3:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C10" s="3">
         <v>49</v>
       </c>
@@ -5893,7 +5893,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="3:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C11" s="3">
         <v>50</v>
       </c>
@@ -5916,7 +5916,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="3:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C12" s="3">
         <v>60</v>
       </c>
@@ -5939,7 +5939,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="3:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C13" s="3">
         <v>70</v>
       </c>
@@ -5962,7 +5962,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="3:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C14" s="3">
         <v>80</v>
       </c>
@@ -5985,7 +5985,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="3:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C15" s="3">
         <v>90</v>
       </c>
@@ -6008,7 +6008,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="3:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C16" s="3">
         <v>99</v>
       </c>
@@ -6031,7 +6031,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="3:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C17" s="3">
         <v>100</v>
       </c>
@@ -6054,7 +6054,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="3:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C18" s="3">
         <v>110</v>
       </c>
@@ -6077,7 +6077,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="3:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C19" s="3">
         <v>120</v>
       </c>
@@ -6100,7 +6100,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="3:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C20" s="3">
         <v>130</v>
       </c>
@@ -6123,7 +6123,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="3:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C21" s="3">
         <v>150</v>
       </c>
@@ -6146,7 +6146,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="3:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C22" s="3">
         <v>200</v>
       </c>
@@ -6169,7 +6169,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="3:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C23" s="3">
         <v>555</v>
       </c>
@@ -6206,18 +6206,17 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="4:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="4:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D7" s="1" t="s">
         <v>14</v>
       </c>
@@ -6228,7 +6227,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="4:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="4:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D8" s="1">
         <v>99</v>
       </c>
@@ -6239,7 +6238,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="4:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="4:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D9" s="1">
         <v>99</v>
       </c>
@@ -6250,7 +6249,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="4:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="4:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D10" s="1">
         <v>99</v>
       </c>
@@ -6261,7 +6260,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="4:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="4:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D11" s="1">
         <v>99</v>
       </c>
@@ -6272,7 +6271,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="4:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="4:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D12" s="1">
         <v>99</v>
       </c>
@@ -6283,7 +6282,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="4:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="4:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D13" s="1">
         <v>99</v>
       </c>
@@ -6294,7 +6293,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="4:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="4:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D14" s="1">
         <v>99</v>
       </c>
@@ -6305,7 +6304,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="4:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="4:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D15" s="1">
         <v>99</v>
       </c>
@@ -6316,7 +6315,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="4:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="16" spans="4:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D16" s="1">
         <v>50</v>
       </c>
@@ -6327,7 +6326,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="4:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D17" s="1">
         <v>50</v>
       </c>

</xml_diff>